<commit_message>
defined recipes, items, materials, started fixing crafting ui
</commit_message>
<xml_diff>
--- a/materials.xlsx
+++ b/materials.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="6735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="6735" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="mats" sheetId="1" r:id="rId1"/>
     <sheet name="effects" sheetId="2" r:id="rId2"/>
+    <sheet name="items" sheetId="3" r:id="rId3"/>
+    <sheet name="recipes" sheetId="4" r:id="rId4"/>
+    <sheet name="recipe_reqs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="93">
   <si>
     <t>WOOD</t>
   </si>
@@ -256,13 +259,61 @@
   </si>
   <si>
     <t>BODY</t>
+  </si>
+  <si>
+    <t>Hide Armor</t>
+  </si>
+  <si>
+    <t>NECK</t>
+  </si>
+  <si>
+    <t>Gold Amulet</t>
+  </si>
+  <si>
+    <t>Silver Amulet</t>
+  </si>
+  <si>
+    <t>RING</t>
+  </si>
+  <si>
+    <t>Brass Ring</t>
+  </si>
+  <si>
+    <t>LEFT_HAND</t>
+  </si>
+  <si>
+    <t>Quarterstaff</t>
+  </si>
+  <si>
+    <t>Iron Sword</t>
+  </si>
+  <si>
+    <t>Bronze Sword</t>
+  </si>
+  <si>
+    <t>Copper Sword</t>
+  </si>
+  <si>
+    <t>extra cap</t>
+  </si>
+  <si>
+    <t>itemname</t>
+  </si>
+  <si>
+    <t>material name</t>
+  </si>
+  <si>
+    <t>recipe item name</t>
+  </si>
+  <si>
+    <t>quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +331,13 @@
       <b/>
       <sz val="9"/>
       <color rgb="FF008000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000080"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -304,12 +362,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -594,12 +655,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="97.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1383,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,8 +1488,8 @@
         <v>76</v>
       </c>
       <c r="E2" t="str">
-        <f>"INSERT INTO `material_effect` (material_id, type, val, slot) VALUES ( (SELECT `id` FROM `material` WHERE `name`='"&amp;A2&amp;"'), '"&amp;B2&amp;"', '"&amp;C2&amp;"', '"&amp;D2&amp;"' )"</f>
-        <v>INSERT INTO `material_effect` (material_id, type, val, slot) VALUES ( (SELECT `id` FROM `material` WHERE `name`='Pine'), 'ADDED_PIERCING_RESIST', '2', 'BODY' )</v>
+        <f>"INSERT INTO `material_effect` (material_id, type, val, slot) VALUES ( (SELECT `id` FROM `material` WHERE `name`='"&amp;A2&amp;"'), '"&amp;B2&amp;"', '"&amp;C2&amp;"', '"&amp;D2&amp;"' );"</f>
+        <v>INSERT INTO `material_effect` (material_id, type, val, slot) VALUES ( (SELECT `id` FROM `material` WHERE `name`='Pine'), 'ADDED_PIERCING_RESIST', '2', 'BODY' );</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1439,323 +1502,813 @@
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E7" si="0">"INSERT INTO `material_effect` (material_id, type, val, slot) VALUES ( (SELECT `id` FROM `material` WHERE `name`='"&amp;A3&amp;"'), '"&amp;B3&amp;"', '"&amp;C3&amp;"', '"&amp;D3&amp;"' );"</f>
+        <v>INSERT INTO `material_effect` (material_id, type, val, slot) VALUES ( (SELECT `id` FROM `material` WHERE `name`='Pine'), 'LESS_FIRE_RESIST', '2', 'BODY' );</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `material_effect` (material_id, type, val, slot) VALUES ( (SELECT `id` FROM `material` WHERE `name`='Fir'), 'ADDED_PIERCING_RESIST', '5', 'BODY' );</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `material_effect` (material_id, type, val, slot) VALUES ( (SELECT `id` FROM `material` WHERE `name`='Fir'), 'LESS_FIRE_RESIST', '5', 'BODY' );</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `material_effect` (material_id, type, val, slot) VALUES ( (SELECT `id` FROM `material` WHERE `name`='Yew'), 'ADDED_PIERCING_RESIST', '10', 'BODY' );</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `material_effect` (material_id, type, val, slot) VALUES ( (SELECT `id` FROM `material` WHERE `name`='Yew'), 'LESS_FIRE_RESIST', '10', 'BODY' );</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="77.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <f>"INSERT INTO `item` (name, body_slot) VALUES ('"&amp;A1&amp;"', '"&amp;B1&amp;"');"</f>
+        <v>INSERT INTO `item` (name, body_slot) VALUES ('Copper Sword', 'LEFT_HAND');</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="3" t="str">
+        <f>"INSERT INTO `item` (name, body_slot) VALUES ('"&amp;A2&amp;"', '"&amp;B2&amp;"');"</f>
+        <v>INSERT INTO `item` (name, body_slot) VALUES ('Bronze Sword', 'LEFT_HAND');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="3" t="str">
+        <f>"INSERT INTO `item` (name, body_slot) VALUES ('"&amp;A3&amp;"', '"&amp;B3&amp;"');"</f>
+        <v>INSERT INTO `item` (name, body_slot) VALUES ('Iron Sword', 'LEFT_HAND');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="3" t="str">
+        <f>"INSERT INTO `item` (name, body_slot) VALUES ('"&amp;A5&amp;"', '"&amp;B5&amp;"');"</f>
+        <v>INSERT INTO `item` (name, body_slot) VALUES ('Quarterstaff', 'LEFT_HAND');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="3" t="str">
+        <f>"INSERT INTO `item` (name, body_slot) VALUES ('"&amp;A7&amp;"', '"&amp;B7&amp;"');"</f>
+        <v>INSERT INTO `item` (name, body_slot) VALUES ('Brass Ring', 'RING');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="3" t="str">
+        <f>"INSERT INTO `item` (name, body_slot) VALUES ('"&amp;A9&amp;"', '"&amp;B9&amp;"');"</f>
+        <v>INSERT INTO `item` (name, body_slot) VALUES ('Silver Amulet', 'NECK');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="3" t="str">
+        <f>"INSERT INTO `item` (name, body_slot) VALUES ('"&amp;A10&amp;"', '"&amp;B10&amp;"');"</f>
+        <v>INSERT INTO `item` (name, body_slot) VALUES ('Gold Amulet', 'NECK');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="3" t="str">
+        <f>"INSERT INTO `item` (name, body_slot) VALUES ('"&amp;A12&amp;"', '"&amp;B12&amp;"');"</f>
+        <v>INSERT INTO `item` (name, body_slot) VALUES ('Hide Armor', 'BODY');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="105.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = '"&amp;A2&amp;"'), '"&amp;B2&amp;"');"</f>
+        <v>INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = 'Copper Sword'), '10');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3" t="str">
+        <f>"INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = '"&amp;A3&amp;"'), '"&amp;B3&amp;"');"</f>
+        <v>INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = 'Bronze Sword'), '15');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4" t="str">
+        <f>"INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = '"&amp;A4&amp;"'), '"&amp;B4&amp;"');"</f>
+        <v>INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = 'Iron Sword'), '20');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" t="str">
+        <f>"INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = '"&amp;A6&amp;"'), '"&amp;B6&amp;"');"</f>
+        <v>INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = 'Quarterstaff'), '10');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="str">
+        <f>"INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = '"&amp;A8&amp;"'), '"&amp;B8&amp;"');"</f>
+        <v>INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = 'Brass Ring'), '7');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="str">
+        <f>"INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = '"&amp;A10&amp;"'), '"&amp;B10&amp;"');"</f>
+        <v>INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = 'Silver Amulet'), '5');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="str">
+        <f>"INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = '"&amp;A11&amp;"'), '"&amp;B11&amp;"');"</f>
+        <v>INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = 'Gold Amulet'), '10');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13" t="str">
+        <f>"INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = '"&amp;A13&amp;"'), '"&amp;B13&amp;"');"</f>
+        <v>INSERT INTO `recipe` (item_id, extra_capacity) VALUES ( (SELECT id FROM item WHERE name = 'Hide Armor'), '15');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F2:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="96.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"INSERT INTO `recipe_requirement` (`material_id`, `recipe_id`, `quantity`) VALUES ( (SELECT id FROM `material` WHERE name = '"&amp;A2&amp;"'), (SELECT r.id FROM `recipe` r JOIN `item` i ON r.item_id = i.id WHERE i.name = '"&amp;B2&amp;"'), '"&amp;C2&amp;"');"</f>
+        <v>INSERT INTO `recipe_requirement` (`material_id`, `recipe_id`, `quantity`) VALUES ( (SELECT id FROM `material` WHERE name = 'Copper'), (SELECT r.id FROM `recipe` r JOIN `item` i ON r.item_id = i.id WHERE i.name = 'Copper Sword'), '3');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F14" si="0">"INSERT INTO `recipe_requirement` (`material_id`, `recipe_id`, `quantity`) VALUES ( (SELECT id FROM `material` WHERE name = '"&amp;A3&amp;"'), (SELECT r.id FROM `recipe` r JOIN `item` i ON r.item_id = i.id WHERE i.name = '"&amp;B3&amp;"'), '"&amp;C3&amp;"');"</f>
+        <v>INSERT INTO `recipe_requirement` (`material_id`, `recipe_id`, `quantity`) VALUES ( (SELECT id FROM `material` WHERE name = 'Copper'), (SELECT r.id FROM `recipe` r JOIN `item` i ON r.item_id = i.id WHERE i.name = 'Bronze Sword'), '2');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `recipe_requirement` (`material_id`, `recipe_id`, `quantity`) VALUES ( (SELECT id FROM `material` WHERE name = 'Tin'), (SELECT r.id FROM `recipe` r JOIN `item` i ON r.item_id = i.id WHERE i.name = 'Bronze Sword'), '2');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `recipe_requirement` (`material_id`, `recipe_id`, `quantity`) VALUES ( (SELECT id FROM `material` WHERE name = 'Iron'), (SELECT r.id FROM `recipe` r JOIN `item` i ON r.item_id = i.id WHERE i.name = 'Iron Sword'), '5');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `recipe_requirement` (`material_id`, `recipe_id`, `quantity`) VALUES ( (SELECT id FROM `material` WHERE name = 'Pine'), (SELECT r.id FROM `recipe` r JOIN `item` i ON r.item_id = i.id WHERE i.name = 'Quarterstaff'), '4');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `recipe_requirement` (`material_id`, `recipe_id`, `quantity`) VALUES ( (SELECT id FROM `material` WHERE name = 'Brass'), (SELECT r.id FROM `recipe` r JOIN `item` i ON r.item_id = i.id WHERE i.name = 'Brass Ring'), '2');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `recipe_requirement` (`material_id`, `recipe_id`, `quantity`) VALUES ( (SELECT id FROM `material` WHERE name = 'Silver'), (SELECT r.id FROM `recipe` r JOIN `item` i ON r.item_id = i.id WHERE i.name = 'Silver Amulet'), '2');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `recipe_requirement` (`material_id`, `recipe_id`, `quantity`) VALUES ( (SELECT id FROM `material` WHERE name = 'Gold'), (SELECT r.id FROM `recipe` r JOIN `item` i ON r.item_id = i.id WHERE i.name = 'Gold Amulet'), '3');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `recipe_requirement` (`material_id`, `recipe_id`, `quantity`) VALUES ( (SELECT id FROM `material` WHERE name = 'Rawhide'), (SELECT r.id FROM `recipe` r JOIN `item` i ON r.item_id = i.id WHERE i.name = 'Hide Armor'), '5');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>